<commit_message>
Same Image Test Case
</commit_message>
<xml_diff>
--- a/Code/Results/Results.xlsx
+++ b/Code/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knaro\Documents\MATLAB\Code\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DCB03-8D2E-4793-A03E-4702FDFD938C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E39487-66BB-4AC5-BDFD-D3D52FBB1264}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14220" xr2:uid="{B5F3582C-0D1B-4472-BED9-A2F61D6E4A8C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="18">
   <si>
     <t>Compression Ratio</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>Simon Matzinger</t>
+  </si>
+  <si>
+    <t>High Contrast Images</t>
+  </si>
+  <si>
+    <t>Ananth Pai</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Yerko Lucic</t>
   </si>
 </sst>
 </file>
@@ -487,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804F6F2C-90E5-40FA-9976-2A57C72B7F44}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -500,16 +512,27 @@
     <col min="4" max="4" width="16.3046875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.61328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.69140625" style="1" customWidth="1"/>
-    <col min="7" max="10" width="9.23046875" style="1"/>
+    <col min="7" max="7" width="9.23046875" style="1"/>
+    <col min="8" max="8" width="4.53515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23046875" style="1"/>
     <col min="11" max="11" width="8.921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.15234375" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.3046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.4609375" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.07421875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.23046875" style="1"/>
+    <col min="16" max="16" width="9.23046875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.07421875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="4.3046875" style="1" customWidth="1"/>
+    <col min="19" max="20" width="9.23046875" style="1"/>
+    <col min="21" max="21" width="18.61328125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="18.07421875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.4609375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11.4609375" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30.9" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:25" ht="30.9" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -528,8 +551,17 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-    </row>
-    <row r="2" spans="1:16" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="S1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+    </row>
+    <row r="2" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -548,8 +580,17 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S2" s="7"/>
+      <c r="T2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="7"/>
+    </row>
+    <row r="3" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -584,8 +625,25 @@
         <v>2</v>
       </c>
       <c r="P3" s="7"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S3" s="7"/>
+      <c r="T3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="7"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
       <c r="B4" s="4">
         <v>0</v>
@@ -620,8 +678,25 @@
         <v>32.550690000000003</v>
       </c>
       <c r="P4" s="7"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S4" s="7"/>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>100</v>
+      </c>
+      <c r="V4" s="4">
+        <v>1.9715</v>
+      </c>
+      <c r="W4" s="9">
+        <v>-12.54121</v>
+      </c>
+      <c r="X4" s="9">
+        <v>17.95234</v>
+      </c>
+      <c r="Y4" s="7"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="4">
         <v>20</v>
@@ -656,8 +731,25 @@
         <v>31.595800000000001</v>
       </c>
       <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S5" s="7"/>
+      <c r="T5" s="4">
+        <v>20</v>
+      </c>
+      <c r="U5" s="4">
+        <v>80</v>
+      </c>
+      <c r="V5" s="4">
+        <v>1.8987000000000001</v>
+      </c>
+      <c r="W5" s="9">
+        <v>-12.22175</v>
+      </c>
+      <c r="X5" s="9">
+        <v>16.679210000000001</v>
+      </c>
+      <c r="Y5" s="7"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6" s="7"/>
       <c r="B6" s="4">
         <v>40</v>
@@ -692,8 +784,25 @@
         <v>27.458179999999999</v>
       </c>
       <c r="P6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S6" s="7"/>
+      <c r="T6" s="4">
+        <v>40</v>
+      </c>
+      <c r="U6" s="4">
+        <v>60</v>
+      </c>
+      <c r="V6" s="5">
+        <v>1.8115000000000001</v>
+      </c>
+      <c r="W6" s="9">
+        <v>-12.27383</v>
+      </c>
+      <c r="X6" s="9">
+        <v>16.880420000000001</v>
+      </c>
+      <c r="Y6" s="7"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7" s="7"/>
       <c r="B7" s="4">
         <v>60</v>
@@ -728,8 +837,25 @@
         <v>26.794740000000001</v>
       </c>
       <c r="P7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S7" s="7"/>
+      <c r="T7" s="4">
+        <v>60</v>
+      </c>
+      <c r="U7" s="4">
+        <v>40</v>
+      </c>
+      <c r="V7" s="5">
+        <v>1.6956</v>
+      </c>
+      <c r="W7" s="9">
+        <v>-11.81305</v>
+      </c>
+      <c r="X7" s="9">
+        <v>15.181179999999999</v>
+      </c>
+      <c r="Y7" s="7"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8" s="7"/>
       <c r="B8" s="4">
         <v>80</v>
@@ -764,20 +890,41 @@
         <v>20.458320000000001</v>
       </c>
       <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S8" s="7"/>
+      <c r="T8" s="4">
+        <v>80</v>
+      </c>
+      <c r="U8" s="4">
+        <v>20</v>
+      </c>
+      <c r="V8" s="5">
+        <v>1.5463</v>
+      </c>
+      <c r="W8" s="9">
+        <v>-11.75187</v>
+      </c>
+      <c r="X8" s="9">
+        <v>14.96881</v>
+      </c>
+      <c r="Y8" s="7"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A9" s="7"/>
       <c r="G9" s="7"/>
       <c r="J9" s="7"/>
       <c r="P9" s="7"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S9" s="7"/>
+      <c r="Y9" s="7"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" s="7"/>
       <c r="G10" s="7"/>
       <c r="J10" s="7"/>
       <c r="P10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="S10" s="7"/>
+      <c r="Y10" s="7"/>
+    </row>
+    <row r="11" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
@@ -796,8 +943,17 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S11" s="7"/>
+      <c r="T11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="7"/>
+    </row>
+    <row r="12" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -832,8 +988,25 @@
         <v>2</v>
       </c>
       <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S12" s="7"/>
+      <c r="T12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="7"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A13" s="7"/>
       <c r="B13" s="4">
         <v>0</v>
@@ -868,8 +1041,25 @@
         <v>40.44256</v>
       </c>
       <c r="P13" s="7"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S13" s="7"/>
+      <c r="T13" s="4">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4">
+        <v>100</v>
+      </c>
+      <c r="V13" s="5">
+        <v>2.6827000000000001</v>
+      </c>
+      <c r="W13" s="9">
+        <v>-21.12387</v>
+      </c>
+      <c r="X13" s="9">
+        <v>129.53489999999999</v>
+      </c>
+      <c r="Y13" s="7"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="4">
         <v>20</v>
@@ -904,8 +1094,25 @@
         <v>44.678629999999998</v>
       </c>
       <c r="P14" s="7"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S14" s="7"/>
+      <c r="T14" s="4">
+        <v>20</v>
+      </c>
+      <c r="U14" s="4">
+        <v>80</v>
+      </c>
+      <c r="V14" s="5">
+        <v>2.6637</v>
+      </c>
+      <c r="W14" s="9">
+        <v>-21.126850000000001</v>
+      </c>
+      <c r="X14" s="9">
+        <v>129.624</v>
+      </c>
+      <c r="Y14" s="7"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
       <c r="B15" s="4">
         <v>40</v>
@@ -940,8 +1147,25 @@
         <v>42.515149999999998</v>
       </c>
       <c r="P15" s="7"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S15" s="7"/>
+      <c r="T15" s="4">
+        <v>40</v>
+      </c>
+      <c r="U15" s="4">
+        <v>60</v>
+      </c>
+      <c r="V15" s="5">
+        <v>2.6217000000000001</v>
+      </c>
+      <c r="W15" s="9">
+        <v>-21.19434</v>
+      </c>
+      <c r="X15" s="9">
+        <v>131.654</v>
+      </c>
+      <c r="Y15" s="7"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>60</v>
@@ -976,8 +1200,25 @@
         <v>38.33963</v>
       </c>
       <c r="P16" s="7"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S16" s="7"/>
+      <c r="T16" s="4">
+        <v>60</v>
+      </c>
+      <c r="U16" s="4">
+        <v>40</v>
+      </c>
+      <c r="V16" s="5">
+        <v>2.5352000000000001</v>
+      </c>
+      <c r="W16" s="9">
+        <v>-21.168389999999999</v>
+      </c>
+      <c r="X16" s="9">
+        <v>130.86959999999999</v>
+      </c>
+      <c r="Y16" s="7"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="4">
         <v>80</v>
@@ -1012,20 +1253,41 @@
         <v>52.81467</v>
       </c>
       <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S17" s="7"/>
+      <c r="T17" s="4">
+        <v>80</v>
+      </c>
+      <c r="U17" s="4">
+        <v>20</v>
+      </c>
+      <c r="V17" s="5">
+        <v>2.4577</v>
+      </c>
+      <c r="W17" s="9">
+        <v>-21.42164</v>
+      </c>
+      <c r="X17" s="9">
+        <v>138.72810000000001</v>
+      </c>
+      <c r="Y17" s="7"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18" s="7"/>
       <c r="G18" s="7"/>
       <c r="J18" s="7"/>
       <c r="P18" s="7"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S18" s="7"/>
+      <c r="Y18" s="7"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A19" s="7"/>
       <c r="G19" s="7"/>
       <c r="J19" s="7"/>
       <c r="P19" s="7"/>
-    </row>
-    <row r="20" spans="1:16" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="S19" s="7"/>
+      <c r="Y19" s="7"/>
+    </row>
+    <row r="20" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -1044,8 +1306,17 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="7"/>
-    </row>
-    <row r="21" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S20" s="7"/>
+      <c r="T20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="7"/>
+    </row>
+    <row r="21" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="7"/>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1080,8 +1351,25 @@
         <v>2</v>
       </c>
       <c r="P21" s="7"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S21" s="7"/>
+      <c r="T21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y21" s="7"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22" s="7"/>
       <c r="B22" s="4">
         <v>0</v>
@@ -1116,8 +1404,25 @@
         <v>70.843850000000003</v>
       </c>
       <c r="P22" s="7"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S22" s="7"/>
+      <c r="T22" s="4">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
+        <v>100</v>
+      </c>
+      <c r="V22" s="5">
+        <v>1.9551000000000001</v>
+      </c>
+      <c r="W22" s="6">
+        <v>-13.543369999999999</v>
+      </c>
+      <c r="X22" s="6">
+        <v>22.611879999999999</v>
+      </c>
+      <c r="Y22" s="7"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A23" s="7"/>
       <c r="B23" s="4">
         <v>20</v>
@@ -1152,8 +1457,25 @@
         <v>82.025760000000005</v>
       </c>
       <c r="P23" s="7"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S23" s="7"/>
+      <c r="T23" s="4">
+        <v>20</v>
+      </c>
+      <c r="U23" s="4">
+        <v>80</v>
+      </c>
+      <c r="V23" s="5">
+        <v>1.9845999999999999</v>
+      </c>
+      <c r="W23" s="6">
+        <v>-14.08756</v>
+      </c>
+      <c r="X23" s="6">
+        <v>25.630410000000001</v>
+      </c>
+      <c r="Y23" s="7"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A24" s="7"/>
       <c r="B24" s="4">
         <v>40</v>
@@ -1188,8 +1510,25 @@
         <v>93.897940000000006</v>
       </c>
       <c r="P24" s="7"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S24" s="7"/>
+      <c r="T24" s="4">
+        <v>40</v>
+      </c>
+      <c r="U24" s="4">
+        <v>60</v>
+      </c>
+      <c r="V24" s="5">
+        <v>1.9883</v>
+      </c>
+      <c r="W24" s="6">
+        <v>-14.00193</v>
+      </c>
+      <c r="X24" s="6">
+        <v>25.130040000000001</v>
+      </c>
+      <c r="Y24" s="7"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A25" s="7"/>
       <c r="B25" s="4">
         <v>60</v>
@@ -1224,8 +1563,25 @@
         <v>92.671279999999996</v>
       </c>
       <c r="P25" s="7"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S25" s="7"/>
+      <c r="T25" s="4">
+        <v>60</v>
+      </c>
+      <c r="U25" s="4">
+        <v>40</v>
+      </c>
+      <c r="V25" s="5">
+        <v>1.9021999999999999</v>
+      </c>
+      <c r="W25" s="6">
+        <v>-14.49466</v>
+      </c>
+      <c r="X25" s="6">
+        <v>28.149180000000001</v>
+      </c>
+      <c r="Y25" s="7"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
       <c r="B26" s="4">
         <v>80</v>
@@ -1260,8 +1616,25 @@
         <v>93.783259999999999</v>
       </c>
       <c r="P26" s="7"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S26" s="7"/>
+      <c r="T26" s="4">
+        <v>80</v>
+      </c>
+      <c r="U26" s="4">
+        <v>20</v>
+      </c>
+      <c r="V26" s="5">
+        <v>1.6492</v>
+      </c>
+      <c r="W26" s="6">
+        <v>-13.05091</v>
+      </c>
+      <c r="X26" s="6">
+        <v>20.18787</v>
+      </c>
+      <c r="Y26" s="7"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="G27" s="7"/>
       <c r="J27" s="7"/>
@@ -1271,12 +1644,19 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1287,7 +1667,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A30" s="7"/>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1306,7 +1686,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" ht="30.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7"/>
       <c r="B31" s="4">
         <v>0</v>
@@ -1325,7 +1705,7 @@
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="7"/>
       <c r="B32" s="4">
         <v>20</v>
@@ -1411,7 +1791,11 @@
       <c r="G36" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="T11:X11"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="K11:O11"/>

</xml_diff>

<commit_message>
Updated Folders, Results and Poster
</commit_message>
<xml_diff>
--- a/Code/Results/Results.xlsx
+++ b/Code/Results/Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knaro\Documents\MATLAB\Code\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81E35AB-D9DF-44D5-9D5D-8BC04FF27575}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C941CB5-CF73-4626-B77E-BD9E6BCE9D37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14220" activeTab="2" xr2:uid="{B5F3582C-0D1B-4472-BED9-A2F61D6E4A8C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14220" activeTab="3" xr2:uid="{B5F3582C-0D1B-4472-BED9-A2F61D6E4A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Same Image Different Sizes" sheetId="1" r:id="rId1"/>
     <sheet name="Different Types of Images" sheetId="2" r:id="rId2"/>
     <sheet name="PSNR_MSE" sheetId="3" r:id="rId3"/>
+    <sheet name="Known Images" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="64">
   <si>
     <t>Compression Ratio</t>
   </si>
@@ -148,6 +149,78 @@
   <si>
     <t>Ones Compliment (High Contrast)</t>
   </si>
+  <si>
+    <t>Compression Depth 8</t>
+  </si>
+  <si>
+    <t>Compression Depth 7</t>
+  </si>
+  <si>
+    <t>Compression Depth 6</t>
+  </si>
+  <si>
+    <t>Compression Depth 5</t>
+  </si>
+  <si>
+    <t>Compression Depth 4</t>
+  </si>
+  <si>
+    <t>Compression Depth 3</t>
+  </si>
+  <si>
+    <t>Compression Depth 2</t>
+  </si>
+  <si>
+    <t>Compression Depth 1</t>
+  </si>
+  <si>
+    <t>Compression Depth 0</t>
+  </si>
+  <si>
+    <t>Landscape Amanda Kerr</t>
+  </si>
+  <si>
+    <t>Camerman</t>
+  </si>
+  <si>
+    <t>Image Compression - DCT 0% error</t>
+  </si>
+  <si>
+    <t>Peppers</t>
+  </si>
+  <si>
+    <t>Mandrill</t>
+  </si>
+  <si>
+    <t>Compressed Image Bits</t>
+  </si>
+  <si>
+    <t>Original Bits</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Image Compression - DWT 10% error</t>
+  </si>
+  <si>
+    <t>Image Compression - DWT 0% error</t>
+  </si>
+  <si>
+    <t>Bit Count</t>
+  </si>
+  <si>
+    <t>Bit Values</t>
+  </si>
+  <si>
+    <t>Image Compression - DCT 10% error</t>
+  </si>
+  <si>
+    <t>Image Compression - Holes 10% error</t>
+  </si>
+  <si>
+    <t>Image Compression - Holes 0% error</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +231,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +250,14 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -285,6 +366,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -302,9 +392,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7055,7 +7168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804F6F2C-90E5-40FA-9976-2A57C72B7F44}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
@@ -7087,61 +7200,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="30.9" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="S1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
     </row>
     <row r="2" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
       <c r="P2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
       <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
@@ -7480,31 +7593,31 @@
     </row>
     <row r="11" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="6"/>
       <c r="S11" s="6"/>
-      <c r="T11" s="8" t="s">
+      <c r="T11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
       <c r="Y11" s="6"/>
     </row>
     <row r="12" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
@@ -7843,31 +7956,31 @@
     </row>
     <row r="20" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="6"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="8" t="s">
+      <c r="T20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
       <c r="Y20" s="6"/>
     </row>
     <row r="21" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
@@ -8212,13 +8325,13 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29" s="6"/>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
@@ -8370,8 +8483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB23DA93-00A6-4BA3-8C16-52BD5176862E}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8383,23 +8496,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.9" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -8452,12 +8565,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -8510,12 +8623,12 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="6"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -8568,12 +8681,12 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -8617,23 +8730,23 @@
       <c r="F20" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="30.9" x14ac:dyDescent="0.8">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="6"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -8686,12 +8799,12 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="6"/>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -8744,12 +8857,12 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="6"/>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -8793,23 +8906,23 @@
       <c r="F37" s="6"/>
     </row>
     <row r="40" spans="1:6" ht="30.9" x14ac:dyDescent="0.8">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="6"/>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -8862,12 +8975,12 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" s="6"/>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
@@ -8920,12 +9033,12 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" s="6"/>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
@@ -8970,22 +9083,23 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A40:F40"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8993,8 +9107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C77634-B01E-4256-B5F7-86C685C48C0B}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9010,1631 +9124,1631 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30.9" x14ac:dyDescent="0.8">
-      <c r="A1" s="15"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="9" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="15"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="15"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="13" t="s">
+      <c r="F2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="15"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="9">
         <v>0</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="11">
         <v>-2.0404740000000001</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="11">
         <v>1.5997319999999999</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="14" t="s">
+      <c r="F3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="9">
         <v>0</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="11">
         <v>-2.0404740000000001</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="11">
         <v>1.5997319999999999</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9">
         <v>20</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="11">
         <v>-16.630230000000001</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="11">
         <v>46.028089999999999</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14">
+      <c r="F4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
         <v>20</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="11">
         <v>-23.694959999999998</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="11">
         <v>234.1508</v>
       </c>
-      <c r="N4" s="15"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="15"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9">
         <v>40</v>
       </c>
-      <c r="D5" s="16">
-        <f>--19.60627</f>
-        <v>19.606269999999999</v>
-      </c>
-      <c r="E5" s="16">
+      <c r="D5" s="11">
+        <f>-19.60627</f>
+        <v>-19.606269999999999</v>
+      </c>
+      <c r="E5" s="11">
         <v>91.332930000000005</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14">
+      <c r="F5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
         <v>40</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="11">
         <v>-26.747969999999999</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="11">
         <v>472.93049999999999</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="15"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
         <v>60</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="11">
         <v>-21.304010000000002</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="11">
         <v>135.02090000000001</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14">
+      <c r="F6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9">
         <v>60</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="11">
         <v>-28.511310000000002</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="11">
         <v>709.79160000000002</v>
       </c>
-      <c r="N6" s="15"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="15"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9">
         <v>80</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="11">
         <v>-22.596589999999999</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="11">
         <v>181.8272</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14">
+      <c r="F7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9">
         <v>80</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="11">
         <v>-29.857399999999998</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="11">
         <v>967.69889999999998</v>
       </c>
-      <c r="N7" s="15"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
         <v>100</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="11">
         <v>-23.61702</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="11">
         <v>229.9862</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14">
+      <c r="F8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
         <v>100</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="11">
         <v>-30.823979999999999</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="11">
         <v>1208.92</v>
       </c>
-      <c r="N8" s="15"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="11">
         <v>10.80522</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="11">
         <v>8.3076440000000001E-2</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="14" t="s">
+      <c r="F9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="9">
         <v>0</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="11">
         <v>10.80522</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="11">
         <v>8.3076440000000001E-2</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9">
         <v>20</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="11">
         <v>-17.46847</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="11">
         <v>55.82734</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14">
+      <c r="F10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9">
         <v>20</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="11">
         <v>-24.077850000000002</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="11">
         <v>255.7321</v>
       </c>
-      <c r="N10" s="15"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14">
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9">
         <v>40</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="11">
         <v>-20.222349999999999</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="11">
         <v>105.2531</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14">
+      <c r="F11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9">
         <v>40</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="11">
         <v>-27.092770000000002</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="11">
         <v>512.00869999999998</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9">
         <v>60</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="11">
         <v>-22.03518</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="11">
         <v>159.7782</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14">
+      <c r="F12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
         <v>60</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="11">
         <v>-28.81063</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="11">
         <v>760.43629999999996</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14">
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
         <v>80</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="11">
         <v>-23.371169999999999</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="11">
         <v>217.32859999999999</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14">
+      <c r="F13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9">
         <v>80</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="11">
         <v>-30.10623</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="11">
         <v>1024.761</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9">
         <v>100</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="11">
         <v>-24.431830000000001</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="11">
         <v>277.44869999999997</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14">
+      <c r="F14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9">
         <v>100</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="11">
         <v>-31.06851</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="11">
         <v>1278.944</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="9">
         <v>0</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="11">
         <v>-3.0726789999999999</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="11">
         <v>2.028934</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14" t="s">
+      <c r="F15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="9">
         <v>0</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="11">
         <v>-3.0726789999999999</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="11">
         <v>2.028934</v>
       </c>
-      <c r="N15" s="15"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14">
+      <c r="A16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9">
         <v>20</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="11">
         <v>-16.656490000000002</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="11">
         <v>46.307250000000003</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14">
+      <c r="F16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9">
         <v>20</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="11">
         <v>-23.64499</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="11">
         <v>231.47219999999999</v>
       </c>
-      <c r="N16" s="15"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14">
+      <c r="A17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9">
         <v>40</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="11">
         <v>-19.576219999999999</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="11">
         <v>90.70308</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14">
+      <c r="F17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9">
         <v>40</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="11">
         <v>-26.633679999999998</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="11">
         <v>460.64690000000002</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14">
+      <c r="A18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9">
         <v>60</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="11">
         <v>-21.373989999999999</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="11">
         <v>137.21420000000001</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14">
+      <c r="F18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9">
         <v>60</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="11">
         <v>-28.41836</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18" s="11">
         <v>694.76189999999997</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14">
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9">
         <v>80</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="11">
         <v>-22.625620000000001</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="11">
         <v>183.04689999999999</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14">
+      <c r="F19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9">
         <v>80</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="11">
         <v>-29.733519999999999</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="11">
         <v>940.48419999999999</v>
       </c>
-      <c r="N19" s="15"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9">
         <v>100</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="11">
         <v>-23.520900000000001</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="11">
         <v>224.952</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14">
+      <c r="F20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9">
         <v>100</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L20" s="11">
         <v>-30.686450000000001</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="11">
         <v>1171.2370000000001</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
     </row>
     <row r="24" spans="1:14" ht="30.9" x14ac:dyDescent="0.8">
-      <c r="A24" s="15"/>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="9" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="15"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="10"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A25" s="15"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="13" t="s">
+      <c r="F25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="13" t="s">
+      <c r="K25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="M25" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="15"/>
+      <c r="N25" s="10"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A26" s="15"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="9">
         <v>0</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="11">
         <v>-3.2704270000000002</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="11">
         <v>2.123453</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="14" t="s">
+      <c r="F26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="9">
         <v>0</v>
       </c>
-      <c r="L26" s="16">
+      <c r="L26" s="11">
         <v>-3.2704270000000002</v>
       </c>
-      <c r="M26" s="16">
+      <c r="M26" s="11">
         <v>2.1234500000000001</v>
       </c>
-      <c r="N26" s="15"/>
+      <c r="N26" s="10"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A27" s="15"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9">
         <v>20</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="11">
         <v>-16.042549999999999</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="11">
         <v>40.202669999999998</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14">
+      <c r="F27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9">
         <v>20</v>
       </c>
-      <c r="L27" s="16">
+      <c r="L27" s="11">
         <v>-23.249929999999999</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="11">
         <v>211.34549999999999</v>
       </c>
-      <c r="N27" s="15"/>
+      <c r="N27" s="10"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A28" s="15"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14">
+      <c r="A28" s="10"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9">
         <v>40</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="11">
         <v>-19.028279999999999</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="11">
         <v>79.951830000000001</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14">
+      <c r="F28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9">
         <v>40</v>
       </c>
-      <c r="L28" s="16">
+      <c r="L28" s="11">
         <v>-26.325310000000002</v>
       </c>
-      <c r="M28" s="16">
+      <c r="M28" s="11">
         <v>429.07240000000002</v>
       </c>
-      <c r="N28" s="15"/>
+      <c r="N28" s="10"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A29" s="15"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14">
+      <c r="A29" s="10"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9">
         <v>60</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="11">
         <v>-20.72289</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="11">
         <v>118.11069999999999</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14">
+      <c r="F29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9">
         <v>60</v>
       </c>
-      <c r="L29" s="16">
+      <c r="L29" s="11">
         <v>-27.999140000000001</v>
       </c>
-      <c r="M29" s="16">
+      <c r="M29" s="11">
         <v>630.83259999999996</v>
       </c>
-      <c r="N29" s="15"/>
+      <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9">
         <v>80</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="11">
         <v>-21.908629999999999</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="11">
         <v>155.18989999999999</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14">
+      <c r="F30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9">
         <v>80</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="11">
         <v>-29.452390000000001</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="11">
         <v>881.53380000000004</v>
       </c>
-      <c r="N30" s="15"/>
+      <c r="N30" s="10"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A31" s="15"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14">
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9">
         <v>100</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="11">
         <v>-22.948060000000002</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="11">
         <v>197.154</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14">
+      <c r="F31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9">
         <v>100</v>
       </c>
-      <c r="L31" s="16">
+      <c r="L31" s="11">
         <v>-30.465920000000001</v>
       </c>
-      <c r="M31" s="16">
+      <c r="M31" s="11">
         <v>1113.248</v>
       </c>
-      <c r="N31" s="15"/>
+      <c r="N31" s="10"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A32" s="15"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="9">
         <v>0</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="11">
         <v>-6.0535480000000002</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="11">
         <v>4.030462</v>
       </c>
-      <c r="F32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="14" t="s">
+      <c r="F32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="9">
         <v>0</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L32" s="11">
         <v>-6.0535480000000002</v>
       </c>
-      <c r="M32" s="16">
+      <c r="M32" s="11">
         <v>4.030462</v>
       </c>
-      <c r="N32" s="15"/>
+      <c r="N32" s="10"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A33" s="15"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14">
+      <c r="A33" s="10"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9">
         <v>20</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="11">
         <v>-17.540420000000001</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="11">
         <v>56.759970000000003</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14">
+      <c r="F33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9">
         <v>20</v>
       </c>
-      <c r="L33" s="16">
+      <c r="L33" s="11">
         <v>-24.477889999999999</v>
       </c>
-      <c r="M33" s="16">
+      <c r="M33" s="11">
         <v>280.40679999999998</v>
       </c>
-      <c r="N33" s="15"/>
+      <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A34" s="15"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14">
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9">
         <v>40</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="11">
         <v>-20.147950000000002</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="11">
         <v>103.4652</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14">
+      <c r="F34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9">
         <v>40</v>
       </c>
-      <c r="L34" s="16">
+      <c r="L34" s="11">
         <v>-27.519760000000002</v>
       </c>
-      <c r="M34" s="16">
+      <c r="M34" s="11">
         <v>564.90570000000002</v>
       </c>
-      <c r="N34" s="15"/>
+      <c r="N34" s="10"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A35" s="15"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14">
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9">
         <v>60</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="11">
         <v>-21.763010000000001</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="11">
         <v>150.07249999999999</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14">
+      <c r="F35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9">
         <v>60</v>
       </c>
-      <c r="L35" s="16">
+      <c r="L35" s="11">
         <v>-29.044129999999999</v>
       </c>
-      <c r="M35" s="16">
+      <c r="M35" s="11">
         <v>802.44039999999995</v>
       </c>
-      <c r="N35" s="15"/>
+      <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A36" s="15"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14">
+      <c r="A36" s="10"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9">
         <v>80</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="11">
         <v>-22.92726</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="11">
         <v>196.2123</v>
       </c>
-      <c r="F36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14">
+      <c r="F36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9">
         <v>80</v>
       </c>
-      <c r="L36" s="16">
+      <c r="L36" s="11">
         <v>-30.42803</v>
       </c>
-      <c r="M36" s="16">
+      <c r="M36" s="11">
         <v>1103.578</v>
       </c>
-      <c r="N36" s="15"/>
+      <c r="N36" s="10"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A37" s="15"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14">
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9">
         <v>100</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="11">
         <v>-23.937419999999999</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="11">
         <v>247.595</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14">
+      <c r="F37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9">
         <v>100</v>
       </c>
-      <c r="L37" s="16">
+      <c r="L37" s="11">
         <v>-31.422529999999998</v>
       </c>
-      <c r="M37" s="16">
+      <c r="M37" s="11">
         <v>1387.5640000000001</v>
       </c>
-      <c r="N37" s="15"/>
+      <c r="N37" s="10"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A38" s="15"/>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="9">
         <v>0</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="11">
         <v>-7.8620960000000002</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="11">
         <v>6.1123690000000002</v>
       </c>
-      <c r="F38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="14" t="s">
+      <c r="F38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="14">
+      <c r="K38" s="9">
         <v>0</v>
       </c>
-      <c r="L38" s="16">
+      <c r="L38" s="11">
         <v>-7.8620960000000002</v>
       </c>
-      <c r="M38" s="16">
+      <c r="M38" s="11">
         <v>6.1123690000000002</v>
       </c>
-      <c r="N38" s="15"/>
+      <c r="N38" s="10"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14">
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9">
         <v>20</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="11">
         <v>-15.76262</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="11">
         <v>37.693080000000002</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14">
+      <c r="F39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9">
         <v>20</v>
       </c>
-      <c r="L39" s="16">
+      <c r="L39" s="11">
         <v>-23.045960000000001</v>
       </c>
-      <c r="M39" s="16">
+      <c r="M39" s="11">
         <v>201.64879999999999</v>
       </c>
-      <c r="N39" s="15"/>
+      <c r="N39" s="10"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A40" s="15"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14">
+      <c r="A40" s="10"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9">
         <v>40</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="11">
         <v>-19.097010000000001</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="11">
         <v>81.227080000000001</v>
       </c>
-      <c r="F40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14">
+      <c r="F40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9">
         <v>40</v>
       </c>
-      <c r="L40" s="16">
+      <c r="L40" s="11">
         <v>-26.107399999999998</v>
       </c>
-      <c r="M40" s="16">
+      <c r="M40" s="11">
         <v>408.07479999999998</v>
       </c>
-      <c r="N40" s="15"/>
+      <c r="N40" s="10"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A41" s="15"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14">
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9">
         <v>60</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="11">
         <v>-20.848109999999998</v>
       </c>
-      <c r="E41" s="16">
+      <c r="E41" s="11">
         <v>121.56570000000001</v>
       </c>
-      <c r="F41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14">
+      <c r="F41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9">
         <v>60</v>
       </c>
-      <c r="L41" s="16">
+      <c r="L41" s="11">
         <v>-28.24091</v>
       </c>
-      <c r="M41" s="16">
+      <c r="M41" s="11">
         <v>666.9461</v>
       </c>
-      <c r="N41" s="15"/>
+      <c r="N41" s="10"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A42" s="15"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14">
+      <c r="A42" s="10"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9">
         <v>80</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="11">
         <v>-21.883769999999998</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E42" s="11">
         <v>154.30410000000001</v>
       </c>
-      <c r="F42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14">
+      <c r="F42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9">
         <v>80</v>
       </c>
-      <c r="L42" s="16">
+      <c r="L42" s="11">
         <v>-29.347850000000001</v>
       </c>
-      <c r="M42" s="16">
+      <c r="M42" s="11">
         <v>860.56730000000005</v>
       </c>
-      <c r="N42" s="15"/>
+      <c r="N42" s="10"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A43" s="15"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14">
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9">
         <v>100</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="11">
         <v>-23.070399999999999</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E43" s="11">
         <v>202.7869</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14">
+      <c r="F43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9">
         <v>100</v>
       </c>
-      <c r="L43" s="16">
+      <c r="L43" s="11">
         <v>-30.37764</v>
       </c>
-      <c r="M43" s="16">
+      <c r="M43" s="11">
         <v>1090.848</v>
       </c>
-      <c r="N43" s="15"/>
+      <c r="N43" s="10"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
     </row>
     <row r="47" spans="1:14" ht="30.9" x14ac:dyDescent="0.8">
-      <c r="A47" s="15"/>
-      <c r="B47" s="9" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="9" t="s">
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="15"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="10"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A48" s="15"/>
-      <c r="B48" s="13" t="s">
+      <c r="A48" s="10"/>
+      <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="13" t="s">
+      <c r="F48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K48" s="13" t="s">
+      <c r="K48" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L48" s="13" t="s">
+      <c r="L48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M48" s="13" t="s">
+      <c r="M48" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N48" s="15"/>
+      <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A49" s="15"/>
-      <c r="B49" s="14" t="s">
+      <c r="A49" s="10"/>
+      <c r="B49" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="9">
         <v>0</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D49" s="11">
         <v>-2.8798780000000002</v>
       </c>
-      <c r="E49" s="16">
+      <c r="E49" s="11">
         <v>1.940831</v>
       </c>
-      <c r="F49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="14" t="s">
+      <c r="F49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K49" s="14">
+      <c r="K49" s="9">
         <v>0</v>
       </c>
-      <c r="L49" s="16">
+      <c r="L49" s="11">
         <v>-2.8798780000000002</v>
       </c>
-      <c r="M49" s="16">
+      <c r="M49" s="11">
         <v>1.940831</v>
       </c>
-      <c r="N49" s="15"/>
+      <c r="N49" s="10"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A50" s="15"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14">
+      <c r="A50" s="10"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9">
         <v>20</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D50" s="11">
         <v>-17.70776</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E50" s="11">
         <v>58.989690000000003</v>
       </c>
-      <c r="F50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14">
+      <c r="F50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9">
         <v>20</v>
       </c>
-      <c r="L50" s="16">
+      <c r="L50" s="11">
         <v>-23.578330000000001</v>
       </c>
-      <c r="M50" s="16">
+      <c r="M50" s="11">
         <v>227.94649999999999</v>
       </c>
-      <c r="N50" s="15"/>
+      <c r="N50" s="10"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A51" s="15"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14">
+      <c r="A51" s="10"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9">
         <v>40</v>
       </c>
-      <c r="D51" s="16">
+      <c r="D51" s="11">
         <v>-20.233979999999999</v>
       </c>
-      <c r="E51" s="16">
+      <c r="E51" s="11">
         <v>105.5355</v>
       </c>
-      <c r="F51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14">
+      <c r="F51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9">
         <v>40</v>
       </c>
-      <c r="L51" s="16">
+      <c r="L51" s="11">
         <v>-26.968129999999999</v>
       </c>
-      <c r="M51" s="16">
+      <c r="M51" s="11">
         <v>497.52249999999998</v>
       </c>
-      <c r="N51" s="15"/>
+      <c r="N51" s="10"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A52" s="15"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14">
+      <c r="A52" s="10"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9">
         <v>60</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="11">
         <v>-22.001110000000001</v>
       </c>
-      <c r="E52" s="16">
+      <c r="E52" s="11">
         <v>158.5299</v>
       </c>
-      <c r="F52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14">
+      <c r="F52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9">
         <v>60</v>
       </c>
-      <c r="L52" s="16">
+      <c r="L52" s="11">
         <v>-28.71857</v>
       </c>
-      <c r="M52" s="16">
+      <c r="M52" s="11">
         <v>744.48620000000005</v>
       </c>
-      <c r="N52" s="15"/>
+      <c r="N52" s="10"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A53" s="15"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14">
+      <c r="A53" s="10"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9">
         <v>80</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D53" s="11">
         <v>-23.37087</v>
       </c>
-      <c r="E53" s="16">
+      <c r="E53" s="11">
         <v>217.3134</v>
       </c>
-      <c r="F53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14">
+      <c r="F53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9">
         <v>80</v>
       </c>
-      <c r="L53" s="16">
+      <c r="L53" s="11">
         <v>-30.218070000000001</v>
       </c>
-      <c r="M53" s="16">
+      <c r="M53" s="11">
         <v>1051.4939999999999</v>
       </c>
-      <c r="N53" s="15"/>
+      <c r="N53" s="10"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A54" s="15"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14">
+      <c r="A54" s="10"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9">
         <v>100</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="11">
         <v>-24.334009999999999</v>
       </c>
-      <c r="E54" s="16">
+      <c r="E54" s="11">
         <v>271.26920000000001</v>
       </c>
-      <c r="F54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14">
+      <c r="F54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9">
         <v>100</v>
       </c>
-      <c r="L54" s="16">
+      <c r="L54" s="11">
         <v>-31.22542</v>
       </c>
-      <c r="M54" s="16">
+      <c r="M54" s="11">
         <v>1325.9960000000001</v>
       </c>
-      <c r="N54" s="15"/>
+      <c r="N54" s="10"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A55" s="15"/>
-      <c r="B55" s="14" t="s">
+      <c r="A55" s="10"/>
+      <c r="B55" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="9">
         <v>0</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="11">
         <v>-8.7808930000000007</v>
       </c>
-      <c r="E55" s="16">
+      <c r="E55" s="11">
         <v>7.5524740000000001</v>
       </c>
-      <c r="F55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="14" t="s">
+      <c r="F55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K55" s="14">
+      <c r="K55" s="9">
         <v>0</v>
       </c>
-      <c r="L55" s="16">
+      <c r="L55" s="11">
         <v>-8.7808930000000007</v>
       </c>
-      <c r="M55" s="16">
+      <c r="M55" s="11">
         <v>7.5524740000000001</v>
       </c>
-      <c r="N55" s="15"/>
+      <c r="N55" s="10"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A56" s="15"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14">
+      <c r="A56" s="10"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9">
         <v>20</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="11">
         <v>-19.189710000000002</v>
       </c>
-      <c r="E56" s="16">
+      <c r="E56" s="11">
         <v>82.979510000000005</v>
       </c>
-      <c r="F56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14">
+      <c r="F56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9">
         <v>20</v>
       </c>
-      <c r="L56" s="16">
+      <c r="L56" s="11">
         <v>-25.55443</v>
       </c>
-      <c r="M56" s="16">
+      <c r="M56" s="11">
         <v>359.28789999999998</v>
       </c>
-      <c r="N56" s="15"/>
+      <c r="N56" s="10"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A57" s="15"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14">
+      <c r="A57" s="10"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9">
         <v>40</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="11">
         <v>-22.126090000000001</v>
       </c>
-      <c r="E57" s="16">
+      <c r="E57" s="11">
         <v>163.1583</v>
       </c>
-      <c r="F57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14">
+      <c r="F57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9">
         <v>40</v>
       </c>
-      <c r="L57" s="16">
+      <c r="L57" s="11">
         <v>-28.547630000000002</v>
       </c>
-      <c r="M57" s="16">
+      <c r="M57" s="11">
         <v>715.75199999999995</v>
       </c>
-      <c r="N57" s="15"/>
+      <c r="N57" s="10"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A58" s="15"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14">
+      <c r="A58" s="10"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9">
         <v>60</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D58" s="11">
         <v>-23.83887</v>
       </c>
-      <c r="E58" s="16">
+      <c r="E58" s="11">
         <v>242.03970000000001</v>
       </c>
-      <c r="F58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14">
+      <c r="F58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9">
         <v>60</v>
       </c>
-      <c r="L58" s="16">
+      <c r="L58" s="11">
         <v>-30.35519</v>
       </c>
-      <c r="M58" s="16">
+      <c r="M58" s="11">
         <v>1085.222</v>
       </c>
-      <c r="N58" s="15"/>
+      <c r="N58" s="10"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A59" s="15"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14">
+      <c r="A59" s="10"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9">
         <v>80</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="11">
         <v>-24.95598</v>
       </c>
-      <c r="E59" s="16">
+      <c r="E59" s="11">
         <v>313.03870000000001</v>
       </c>
-      <c r="F59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14">
+      <c r="F59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9">
         <v>80</v>
       </c>
-      <c r="L59" s="16">
+      <c r="L59" s="11">
         <v>-31.556609999999999</v>
       </c>
-      <c r="M59" s="16">
+      <c r="M59" s="11">
         <v>1431.0709999999999</v>
       </c>
-      <c r="N59" s="15"/>
+      <c r="N59" s="10"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A60" s="15"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14">
+      <c r="A60" s="10"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9">
         <v>100</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="11">
         <v>-26.038329999999998</v>
       </c>
-      <c r="E60" s="16">
+      <c r="E60" s="11">
         <v>401.63630000000001</v>
       </c>
-      <c r="F60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14">
+      <c r="F60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9">
         <v>100</v>
       </c>
-      <c r="L60" s="16">
+      <c r="L60" s="11">
         <v>-32.501649999999998</v>
       </c>
-      <c r="M60" s="16">
+      <c r="M60" s="11">
         <v>1778.954</v>
       </c>
-      <c r="N60" s="15"/>
+      <c r="N60" s="10"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A61" s="15"/>
-      <c r="B61" s="14" t="s">
+      <c r="A61" s="10"/>
+      <c r="B61" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="9">
         <v>0</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="11">
         <v>-10.17815</v>
       </c>
-      <c r="E61" s="16">
+      <c r="E61" s="11">
         <v>10.418749999999999</v>
       </c>
-      <c r="F61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="14" t="s">
+      <c r="F61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K61" s="14">
+      <c r="K61" s="9">
         <v>0</v>
       </c>
-      <c r="L61" s="16">
+      <c r="L61" s="11">
         <v>-10.17815</v>
       </c>
-      <c r="M61" s="16">
+      <c r="M61" s="11">
         <v>10.418749999999999</v>
       </c>
-      <c r="N61" s="15"/>
+      <c r="N61" s="10"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A62" s="15"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14">
+      <c r="A62" s="10"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9">
         <v>20</v>
       </c>
-      <c r="D62" s="16">
+      <c r="D62" s="11">
         <v>-17.907350000000001</v>
       </c>
-      <c r="E62" s="16">
+      <c r="E62" s="11">
         <v>61.763959999999997</v>
       </c>
-      <c r="F62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14">
+      <c r="F62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9">
         <v>20</v>
       </c>
-      <c r="L62" s="16">
+      <c r="L62" s="11">
         <v>-24.17679</v>
       </c>
-      <c r="M62" s="16">
+      <c r="M62" s="11">
         <v>261.625</v>
       </c>
-      <c r="N62" s="15"/>
+      <c r="N62" s="10"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A63" s="15"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14">
+      <c r="A63" s="10"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9">
         <v>40</v>
       </c>
-      <c r="D63" s="16">
+      <c r="D63" s="11">
         <v>-20.799910000000001</v>
       </c>
-      <c r="E63" s="16">
+      <c r="E63" s="11">
         <v>120.22410000000001</v>
       </c>
-      <c r="F63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14">
+      <c r="F63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9">
         <v>40</v>
       </c>
-      <c r="L63" s="16">
+      <c r="L63" s="11">
         <v>-26.8217</v>
       </c>
-      <c r="M63" s="16">
+      <c r="M63" s="11">
         <v>481.02890000000002</v>
       </c>
-      <c r="N63" s="15"/>
+      <c r="N63" s="10"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A64" s="15"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14">
+      <c r="A64" s="10"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9">
         <v>60</v>
       </c>
-      <c r="D64" s="16">
+      <c r="D64" s="11">
         <v>-22.06758</v>
       </c>
-      <c r="E64" s="16">
+      <c r="E64" s="11">
         <v>160.97470000000001</v>
       </c>
-      <c r="F64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14">
+      <c r="F64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9">
         <v>60</v>
       </c>
-      <c r="L64" s="16">
+      <c r="L64" s="11">
         <v>-28.92623</v>
       </c>
-      <c r="M64" s="16">
+      <c r="M64" s="11">
         <v>780.94989999999996</v>
       </c>
-      <c r="N64" s="15"/>
+      <c r="N64" s="10"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A65" s="15"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14">
+      <c r="A65" s="10"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9">
         <v>80</v>
       </c>
-      <c r="D65" s="16">
+      <c r="D65" s="11">
         <v>-23.692</v>
       </c>
-      <c r="E65" s="16">
+      <c r="E65" s="11">
         <v>233.9915</v>
       </c>
-      <c r="F65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14">
+      <c r="F65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9">
         <v>80</v>
       </c>
-      <c r="L65" s="16">
+      <c r="L65" s="11">
         <v>-30.163499999999999</v>
       </c>
-      <c r="M65" s="16">
+      <c r="M65" s="11">
         <v>1038.365</v>
       </c>
-      <c r="N65" s="15"/>
+      <c r="N65" s="10"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A66" s="15"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14">
+      <c r="A66" s="10"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9">
         <v>100</v>
       </c>
-      <c r="D66" s="16">
+      <c r="D66" s="11">
         <v>-24.441980000000001</v>
       </c>
-      <c r="E66" s="16">
+      <c r="E66" s="11">
         <v>278.09780000000001</v>
       </c>
-      <c r="F66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14">
+      <c r="F66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9">
         <v>100</v>
       </c>
-      <c r="L66" s="16">
+      <c r="L66" s="11">
         <v>-31.22878</v>
       </c>
-      <c r="M66" s="16">
+      <c r="M66" s="11">
         <v>1327.0219999999999</v>
       </c>
-      <c r="N66" s="15"/>
+      <c r="N66" s="10"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A67" s="15"/>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -10648,4 +10762,1009 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08ABAB0-0A28-4F26-8FF3-44E886F00CAF}">
+  <dimension ref="A1:Q32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="16.23046875" customWidth="1"/>
+    <col min="3" max="3" width="19.61328125" customWidth="1"/>
+    <col min="4" max="4" width="10.69140625" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.4609375" customWidth="1"/>
+    <col min="11" max="11" width="17.84375" customWidth="1"/>
+    <col min="12" max="12" width="11.15234375" customWidth="1"/>
+    <col min="13" max="13" width="11.3046875" customWidth="1"/>
+    <col min="14" max="14" width="14.3828125" customWidth="1"/>
+    <col min="15" max="15" width="13.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A3" s="10"/>
+      <c r="B3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0.98070000000000002</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.26260159999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.94132550000000004</v>
+      </c>
+      <c r="F4" s="21">
+        <v>2097152</v>
+      </c>
+      <c r="G4" s="21">
+        <v>1876712</v>
+      </c>
+      <c r="H4" s="9">
+        <v>261757</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="L4" s="5">
+        <v>-13.723229999999999</v>
+      </c>
+      <c r="M4" s="5">
+        <v>23.56804</v>
+      </c>
+      <c r="N4" s="21">
+        <v>2097152</v>
+      </c>
+      <c r="O4" s="9">
+        <v>1875783</v>
+      </c>
+      <c r="P4" s="9">
+        <v>261757</v>
+      </c>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A5" s="10"/>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1.0984</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-12.02183</v>
+      </c>
+      <c r="E5" s="5">
+        <v>15.928800000000001</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2097152</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1652908</v>
+      </c>
+      <c r="H5" s="9">
+        <v>256410</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="26">
+        <v>1.0989</v>
+      </c>
+      <c r="L5" s="5">
+        <v>-15.69462</v>
+      </c>
+      <c r="M5" s="5">
+        <v>37.107489999999999</v>
+      </c>
+      <c r="N5" s="9">
+        <v>2097152</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1652052</v>
+      </c>
+      <c r="P5" s="9">
+        <v>256410</v>
+      </c>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" s="10"/>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="26">
+        <v>1.3797999999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-9.5975169999999999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>9.1148950000000006</v>
+      </c>
+      <c r="F6" s="9">
+        <v>524288</v>
+      </c>
+      <c r="G6" s="9">
+        <v>322343</v>
+      </c>
+      <c r="H6" s="9">
+        <v>57643</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="26">
+        <v>1.3807</v>
+      </c>
+      <c r="L6" s="5">
+        <v>-15.37074</v>
+      </c>
+      <c r="M6" s="5">
+        <v>34.440849999999998</v>
+      </c>
+      <c r="N6" s="9">
+        <v>524288</v>
+      </c>
+      <c r="O6" s="9">
+        <v>322088</v>
+      </c>
+      <c r="P6" s="9">
+        <v>57643</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A8" s="10"/>
+      <c r="B8" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" s="10"/>
+      <c r="B9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="D10" s="26">
+        <v>-42.658999999999999</v>
+      </c>
+      <c r="E10" s="27">
+        <v>17652</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2097152</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1872657</v>
+      </c>
+      <c r="H10" s="9">
+        <v>261412</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="26">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="L10" s="26">
+        <v>5.7374999999999998</v>
+      </c>
+      <c r="M10" s="26">
+        <v>0.26679999999999998</v>
+      </c>
+      <c r="N10" s="21">
+        <v>2097152</v>
+      </c>
+      <c r="O10" s="9">
+        <v>1872657</v>
+      </c>
+      <c r="P10" s="9">
+        <v>261412</v>
+      </c>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A11" s="10"/>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="26">
+        <v>1.0932999999999999</v>
+      </c>
+      <c r="D11" s="26">
+        <v>-42.360199999999999</v>
+      </c>
+      <c r="E11" s="27">
+        <v>17219</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2097152</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1660986</v>
+      </c>
+      <c r="H11" s="9">
+        <v>257233</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="26">
+        <v>1.0932999999999999</v>
+      </c>
+      <c r="L11" s="26">
+        <v>4.9020000000000001</v>
+      </c>
+      <c r="M11" s="26">
+        <v>0.32340000000000002</v>
+      </c>
+      <c r="N11" s="9">
+        <v>2097152</v>
+      </c>
+      <c r="O11" s="9">
+        <v>1660986</v>
+      </c>
+      <c r="P11" s="9">
+        <v>257233</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A12" s="10"/>
+      <c r="B12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="26">
+        <v>1.2116</v>
+      </c>
+      <c r="D12" s="26">
+        <v>-42.514400000000002</v>
+      </c>
+      <c r="E12" s="27">
+        <v>17842</v>
+      </c>
+      <c r="F12" s="9">
+        <v>524288</v>
+      </c>
+      <c r="G12" s="9">
+        <v>370489</v>
+      </c>
+      <c r="H12" s="9">
+        <v>62249</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="26">
+        <v>1.2116</v>
+      </c>
+      <c r="L12" s="26">
+        <v>4.6393000000000004</v>
+      </c>
+      <c r="M12" s="26">
+        <v>0.34360000000000002</v>
+      </c>
+      <c r="N12" s="9">
+        <v>524288</v>
+      </c>
+      <c r="O12" s="9">
+        <v>370489</v>
+      </c>
+      <c r="P12" s="9">
+        <v>62249</v>
+      </c>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" s="10"/>
+      <c r="B14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="10"/>
+    </row>
+    <row r="15" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A15" s="10"/>
+      <c r="B15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="26">
+        <v>7.0533999999999999</v>
+      </c>
+      <c r="D16" s="26">
+        <v>35.013100000000001</v>
+      </c>
+      <c r="E16" s="26">
+        <v>20.500599999999999</v>
+      </c>
+      <c r="F16" s="21">
+        <v>793302</v>
+      </c>
+      <c r="G16" s="9">
+        <v>15828</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="26">
+        <v>7.0533999999999999</v>
+      </c>
+      <c r="L16" s="26">
+        <v>25.252199999999998</v>
+      </c>
+      <c r="M16" s="26">
+        <v>194.0265</v>
+      </c>
+      <c r="N16" s="21">
+        <v>793302</v>
+      </c>
+      <c r="O16" s="9">
+        <v>15828</v>
+      </c>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="10"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A17" s="10"/>
+      <c r="B17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="26">
+        <v>10.2502</v>
+      </c>
+      <c r="D17" s="26">
+        <v>34.853999999999999</v>
+      </c>
+      <c r="E17" s="26">
+        <v>21.265699999999999</v>
+      </c>
+      <c r="F17" s="9">
+        <v>793298</v>
+      </c>
+      <c r="G17" s="9">
+        <v>74418</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="26">
+        <v>10.2502</v>
+      </c>
+      <c r="L17" s="26">
+        <v>24.9986</v>
+      </c>
+      <c r="M17" s="26">
+        <v>205.69159999999999</v>
+      </c>
+      <c r="N17" s="9">
+        <v>793298</v>
+      </c>
+      <c r="O17" s="9">
+        <v>74418</v>
+      </c>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A18" s="10"/>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="26">
+        <v>66.188000000000002</v>
+      </c>
+      <c r="D18" s="26">
+        <v>35.120100000000001</v>
+      </c>
+      <c r="E18" s="26">
+        <v>20.001999999999999</v>
+      </c>
+      <c r="F18" s="9">
+        <v>65126</v>
+      </c>
+      <c r="G18" s="9">
+        <v>1286</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="26">
+        <v>66.188000000000002</v>
+      </c>
+      <c r="L18" s="26">
+        <v>25.4041</v>
+      </c>
+      <c r="M18" s="26">
+        <v>187.357</v>
+      </c>
+      <c r="N18" s="9">
+        <v>65126</v>
+      </c>
+      <c r="O18" s="9">
+        <v>1286</v>
+      </c>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="10"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A20" s="10"/>
+      <c r="B20" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="26">
+        <v>12.8</v>
+      </c>
+      <c r="D23" s="26">
+        <v>2.47E-2</v>
+      </c>
+      <c r="E23" s="26">
+        <v>0.99429999999999996</v>
+      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26">
+        <v>12.8</v>
+      </c>
+      <c r="H23" s="26">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="I23" s="26">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="26">
+        <v>5.7777000000000003</v>
+      </c>
+      <c r="D24" s="26">
+        <v>4.7645999999999997</v>
+      </c>
+      <c r="E24" s="26">
+        <v>0.33379999999999999</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="26">
+        <v>6.0842999999999998</v>
+      </c>
+      <c r="H24" s="26">
+        <v>3.2366999999999999</v>
+      </c>
+      <c r="I24" s="26">
+        <v>0.47460000000000002</v>
+      </c>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="26">
+        <v>1.6132</v>
+      </c>
+      <c r="D25" s="26">
+        <v>4.6997999999999998</v>
+      </c>
+      <c r="E25" s="26">
+        <v>0.33889999999999998</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="26">
+        <v>1.46</v>
+      </c>
+      <c r="H25" s="26">
+        <v>3.2218</v>
+      </c>
+      <c r="I25" s="26">
+        <v>0.47620000000000001</v>
+      </c>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="10"/>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="26">
+        <v>1.4036</v>
+      </c>
+      <c r="D26" s="28">
+        <v>4.6726000000000001</v>
+      </c>
+      <c r="E26" s="28">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="26">
+        <v>1.3285</v>
+      </c>
+      <c r="H26" s="26">
+        <v>3.2134999999999998</v>
+      </c>
+      <c r="I26" s="26">
+        <v>0.47710000000000002</v>
+      </c>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="10"/>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="28">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="D27" s="28">
+        <v>4.6513999999999998</v>
+      </c>
+      <c r="E27" s="28">
+        <v>0.3427</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="26">
+        <v>1.2921</v>
+      </c>
+      <c r="H27" s="26">
+        <v>3.2092000000000001</v>
+      </c>
+      <c r="I27" s="26">
+        <v>0.47760000000000002</v>
+      </c>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A28" s="10"/>
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="28">
+        <v>1.2116</v>
+      </c>
+      <c r="D28" s="28">
+        <v>4.6436000000000002</v>
+      </c>
+      <c r="E28" s="28">
+        <v>0.34329999999999999</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="26">
+        <v>1.2804</v>
+      </c>
+      <c r="H28" s="26">
+        <v>3.2080000000000002</v>
+      </c>
+      <c r="I28" s="26">
+        <v>0.47770000000000001</v>
+      </c>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A29" s="10"/>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="28">
+        <v>1.1608000000000001</v>
+      </c>
+      <c r="D29" s="28">
+        <v>4.6334</v>
+      </c>
+      <c r="E29" s="28">
+        <v>0.34410000000000002</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="26">
+        <v>1.2773000000000001</v>
+      </c>
+      <c r="H29" s="26">
+        <v>3.2069000000000001</v>
+      </c>
+      <c r="I29" s="26">
+        <v>0.47789999999999999</v>
+      </c>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A30" s="10"/>
+      <c r="B30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="28">
+        <v>1.1288</v>
+      </c>
+      <c r="D30" s="28">
+        <v>4.6269</v>
+      </c>
+      <c r="E30" s="28">
+        <v>0.34460000000000002</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="26">
+        <v>1.2765</v>
+      </c>
+      <c r="H30" s="26">
+        <v>3.2057000000000002</v>
+      </c>
+      <c r="I30" s="26">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="10"/>
+      <c r="B31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="28">
+        <v>1.1238999999999999</v>
+      </c>
+      <c r="D31" s="28">
+        <v>4.6215000000000002</v>
+      </c>
+      <c r="E31" s="28">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="26">
+        <v>1.2762</v>
+      </c>
+      <c r="H31" s="26">
+        <v>3.2029000000000001</v>
+      </c>
+      <c r="I31" s="26">
+        <v>0.4783</v>
+      </c>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>